<commit_message>
added results from CANACE8C
</commit_message>
<xml_diff>
--- a/Documents/Bootloader/extended message by module.xlsx
+++ b/Documents/Bootloader/extended message by module.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\source\repos\david284\MMC-SERVER\Documents\Bootloader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E760DD5A-3678-4926-85E7-75D7E8C27A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F7C8F2-A8A0-43A1-8297-D851B47A762C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>SPCMD_NOP</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>Version 3d</t>
+  </si>
+  <si>
+    <t>CANACE8C</t>
+  </si>
+  <si>
+    <t>Version 2q</t>
   </si>
 </sst>
 </file>
@@ -409,36 +415,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="16.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.73046875" customWidth="1"/>
-    <col min="4" max="4" width="13.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.73046875" customWidth="1"/>
+    <col min="5" max="5" width="13.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C1" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -446,7 +458,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -456,8 +468,11 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -465,6 +480,9 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>